<commit_message>
feat: Refine historical review and switch to live Google Sheet data
</commit_message>
<xml_diff>
--- a/data/balancesheet_2425.xlsx
+++ b/data/balancesheet_2425.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusiyao/Desktop/VT/clubtennis2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{009E8F9D-8D78-5542-83CF-9D1CDEE3441B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DCD841-2825-D143-8597-67FE17A4D8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="1020" windowWidth="30220" windowHeight="17040" xr2:uid="{826D07C5-0512-774F-818D-C92BC356ACDF}"/>
+    <workbookView xWindow="0" yWindow="3020" windowWidth="30220" windowHeight="17040" xr2:uid="{826D07C5-0512-774F-818D-C92BC356ACDF}"/>
   </bookViews>
   <sheets>
     <sheet name="FY 24-25" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="226">
   <si>
     <t>Date</t>
   </si>
@@ -675,16 +675,72 @@
   </si>
   <si>
     <t>F0139558</t>
+  </si>
+  <si>
+    <t>fund balance 24-25</t>
+  </si>
+  <si>
+    <t>allocation 04/25-06/25</t>
+  </si>
+  <si>
+    <t>FJ080252</t>
+  </si>
+  <si>
+    <t>University  of Tennessee</t>
+  </si>
+  <si>
+    <t>canceled check; P4584020</t>
+  </si>
+  <si>
+    <t>C3241623</t>
+  </si>
+  <si>
+    <t>*check needs to be reissued to another entity</t>
+  </si>
+  <si>
+    <t>Kaitlin Ly</t>
+  </si>
+  <si>
+    <t>Tournament entry fee from (3/1-3/2)</t>
+  </si>
+  <si>
+    <t>P4658883</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Penn Tennis Balls </t>
+  </si>
+  <si>
+    <t>Spring Invitational Team Entry Fee</t>
+  </si>
+  <si>
+    <t>EStimate</t>
+  </si>
+  <si>
+    <t>Team Uniforms</t>
+  </si>
+  <si>
+    <t>ESTIMATe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joshua Padgett (180) </t>
+  </si>
+  <si>
+    <t>2x12 passenger van from 9/19-9/21 for travel to College Park, MD (227909, 227908)</t>
+  </si>
+  <si>
+    <t>2x12 passenger van from 9/26-9/28 for travel to Charlottesville, VA (227985,227986)</t>
+  </si>
+  <si>
+    <t>1x12 passanger van from 10/3-10/5 for travel to Boyds, MD (227907)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -847,17 +903,17 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1206,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE57724-7E20-584E-B475-35369E50354B}">
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" x14ac:dyDescent="0.25"/>
@@ -4223,69 +4279,335 @@
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="16">
+        <v>45839</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="F111" s="2">
-        <f t="shared" si="1"/>
-        <v>18674.399999999994</v>
+        <v>18674.400000000001</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="17">
+        <v>45866</v>
+      </c>
+      <c r="B112" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C112" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D112" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="E112" s="21">
+        <v>10</v>
+      </c>
       <c r="F112" s="2">
-        <f t="shared" si="1"/>
-        <v>18674.399999999994</v>
-      </c>
-    </row>
-    <row r="113" spans="6:6" x14ac:dyDescent="0.25">
+        <f>F111+E112</f>
+        <v>18684.400000000001</v>
+      </c>
+      <c r="G112" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="16">
+        <v>45862</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E113" s="19">
+        <v>350</v>
+      </c>
       <c r="F113" s="2">
-        <f t="shared" si="1"/>
-        <v>18674.399999999994</v>
-      </c>
-    </row>
-    <row r="114" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F113:F133" si="2">F112+E113</f>
+        <v>19034.400000000001</v>
+      </c>
+      <c r="G113" s="1">
+        <v>12211</v>
+      </c>
+      <c r="H113" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="16">
+        <v>45890</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E114" s="19">
+        <v>-350</v>
+      </c>
       <c r="F114" s="2">
-        <f t="shared" si="1"/>
-        <v>18674.399999999994</v>
-      </c>
-    </row>
-    <row r="115" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>18684.400000000001</v>
+      </c>
+      <c r="G114" s="1">
+        <v>12211</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="16">
+        <v>45895</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E115" s="19">
+        <v>-139.96</v>
+      </c>
       <c r="F115" s="2">
-        <f t="shared" si="1"/>
-        <v>18674.399999999994</v>
-      </c>
-    </row>
-    <row r="116" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>18544.440000000002</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="16">
+        <v>45912</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E116" s="19">
+        <v>-200</v>
+      </c>
       <c r="F116" s="2">
-        <f t="shared" si="1"/>
-        <v>18674.399999999994</v>
-      </c>
-    </row>
-    <row r="117" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>18344.440000000002</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="16">
+        <v>45915</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E117" s="19">
+        <v>-14476.16</v>
+      </c>
       <c r="F117" s="2">
-        <f t="shared" si="1"/>
-        <v>18674.399999999994</v>
-      </c>
-    </row>
-    <row r="118" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>3868.2800000000025</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="16">
+        <v>45918</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E118" s="19">
+        <v>180</v>
+      </c>
       <c r="F118" s="2">
-        <f t="shared" si="1"/>
-        <v>18674.399999999994</v>
-      </c>
-    </row>
-    <row r="119" spans="6:6" x14ac:dyDescent="0.25">
+        <f>F120+E118</f>
+        <v>2650.4800000000023</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="42" x14ac:dyDescent="0.25">
+      <c r="A119" s="16">
+        <v>45919</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C119" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E119" s="19">
+        <v>-464.4</v>
+      </c>
       <c r="F119" s="2">
-        <f t="shared" si="1"/>
-        <v>18674.399999999994</v>
-      </c>
-    </row>
-    <row r="120" spans="6:6" x14ac:dyDescent="0.25">
+        <f>F117+E119</f>
+        <v>3403.8800000000024</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="16">
+        <v>45919</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E120" s="19">
+        <v>180</v>
+      </c>
       <c r="F120" s="2">
-        <f t="shared" si="1"/>
-        <v>18674.399999999994</v>
-      </c>
-    </row>
-    <row r="121" spans="6:6" x14ac:dyDescent="0.25">
+        <f>F122+E120</f>
+        <v>2470.4800000000023</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="42" x14ac:dyDescent="0.25">
+      <c r="A121" s="16">
+        <v>45926</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E121" s="19">
+        <v>-848</v>
+      </c>
       <c r="F121" s="2">
-        <f t="shared" ref="F121" si="2">F120+E121</f>
-        <v>18674.399999999994</v>
+        <f>F119+E121</f>
+        <v>2555.8800000000024</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="42" x14ac:dyDescent="0.25">
+      <c r="A122" s="16">
+        <v>45933</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C122" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E122" s="19">
+        <v>-265.39999999999998</v>
+      </c>
+      <c r="F122" s="2">
+        <f t="shared" si="2"/>
+        <v>2290.4800000000023</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F123" s="2">
+        <f>F118+E123</f>
+        <v>2650.4800000000023</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F124" s="2">
+        <f t="shared" si="2"/>
+        <v>2650.4800000000023</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F125" s="2">
+        <f t="shared" si="2"/>
+        <v>2650.4800000000023</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F126" s="2">
+        <f t="shared" si="2"/>
+        <v>2650.4800000000023</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F127" s="2">
+        <f t="shared" si="2"/>
+        <v>2650.4800000000023</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F128" s="2">
+        <f t="shared" si="2"/>
+        <v>2650.4800000000023</v>
+      </c>
+    </row>
+    <row r="129" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F129" s="2">
+        <f t="shared" si="2"/>
+        <v>2650.4800000000023</v>
+      </c>
+    </row>
+    <row r="130" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F130" s="2">
+        <f t="shared" si="2"/>
+        <v>2650.4800000000023</v>
+      </c>
+    </row>
+    <row r="131" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F131" s="2">
+        <f t="shared" si="2"/>
+        <v>2650.4800000000023</v>
+      </c>
+    </row>
+    <row r="132" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F132" s="2">
+        <f t="shared" si="2"/>
+        <v>2650.4800000000023</v>
+      </c>
+    </row>
+    <row r="133" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F133" s="2">
+        <f t="shared" si="2"/>
+        <v>2650.4800000000023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>